<commit_message>
DA 19 | Day 10 Complete
</commit_message>
<xml_diff>
--- a/Batch/19/Day_1_PS.xlsx
+++ b/Batch/19/Day_1_PS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive\Work\Acciojob\Modules\Excel\Batch\19\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive\Work\Acciojob\Modules\excel\Batch\19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF828014-B8BF-4E5C-A39D-1FF1DAFEB0C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E930CA9-CF9E-4B87-8978-2B2BC4712CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1071,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5269215-0B5A-4984-A971-F2CC3EAEEBE4}">
   <dimension ref="B1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>